<commit_message>
many many bug fixes and a reasonable set of lifemap specs
</commit_message>
<xml_diff>
--- a/rufus/carriers/lifemap_science/order/biotime_purchase_type.xlsx
+++ b/rufus/carriers/lifemap_science/order/biotime_purchase_type.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2060" yWindow="0" windowWidth="31760" windowHeight="15800" tabRatio="500"/>
+    <workbookView xWindow="3600" yWindow="0" windowWidth="33800" windowHeight="12260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -69,9 +69,6 @@
     <t>$("Human Embryonic Stem Cell", "Human Embryonic Progenitor")</t>
   </si>
   <si>
-    <t>in:pkg_qty</t>
-  </si>
-  <si>
     <t>in:total_quantity</t>
   </si>
   <si>
@@ -87,20 +84,23 @@
     <t>2 day</t>
   </si>
   <si>
-    <t>$in intersection $("Differentiation Kit" "Human Embryonic Progenitor Package" "Growth Media" "Basal Media") #&gt; 0</t>
-  </si>
-  <si>
     <t>$(BioTime)</t>
   </si>
   <si>
     <t>in:vendor_set</t>
+  </si>
+  <si>
+    <t>$in intersection $(Differentiation Kit, Human Embryonic Progenitor Package, Growth Media, Basal Media) #&gt; 0</t>
+  </si>
+  <si>
+    <t>in:pkg_quantity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -146,8 +146,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="72"/>
+      <name val="Lucida Grande"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -163,6 +168,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -185,7 +196,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="73">
+  <cellStyleXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -259,8 +270,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -271,8 +286,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="73">
+  <cellStyles count="77">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -309,6 +325,8 @@
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -345,11 +363,80 @@
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>127000</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>76200</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>1054100</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>431800</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1025" name="Button 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1025"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:latin typeface="Calibri"/>
+                  <a:ea typeface="Calibri"/>
+                  <a:cs typeface="Calibri"/>
+                </a:rPr>
+                <a:t>Run!</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData fPrintsWithSheet="0"/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -673,11 +760,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -689,32 +777,33 @@
     <col min="5" max="7" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" ht="39" customHeight="1">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="B1" s="10"/>
     </row>
     <row r="2" spans="1:12" s="3" customFormat="1">
       <c r="A2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>10</v>
@@ -734,7 +823,7 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -769,7 +858,7 @@
     </row>
     <row r="4" spans="1:12" ht="16" thickBot="1">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -804,10 +893,10 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>8</v>
@@ -840,17 +929,17 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F6" s="6">
         <v>0</v>
@@ -876,10 +965,10 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>9</v>
@@ -912,17 +1001,17 @@
     </row>
     <row r="8" spans="1:12" ht="16" thickBot="1">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F8" s="6">
         <v>0</v>
@@ -948,7 +1037,7 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>7</v>
@@ -984,7 +1073,7 @@
     </row>
     <row r="10" spans="1:12" ht="16" thickBot="1">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -1019,7 +1108,7 @@
     </row>
     <row r="11" spans="1:12" ht="16" thickBot="1">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>15</v>
@@ -1051,12 +1140,12 @@
         <v>5900</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" ht="16" thickBot="1">
       <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>23</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>22</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="8" t="s">
@@ -1089,10 +1178,10 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>23</v>
-      </c>
-      <c r="B13" t="s">
-        <v>22</v>
       </c>
       <c r="D13" t="s">
         <v>9</v>
@@ -1125,6 +1214,38 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1025" r:id="rId3" name="Button 1">
+              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[0]!RunDecisions">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>127000</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>76200</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>1054100</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>431800</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+          <mc:Fallback/>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
combo order working after endless debugging
</commit_message>
<xml_diff>
--- a/rufus/carriers/lifemap_science/order/biotime_purchase_type.xlsx
+++ b/rufus/carriers/lifemap_science/order/biotime_purchase_type.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3600" yWindow="0" windowWidth="33800" windowHeight="12260" tabRatio="500"/>
+    <workbookView xWindow="-38360" yWindow="-440" windowWidth="38360" windowHeight="11480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,6 @@
     <t>Overnight</t>
   </si>
   <si>
-    <t>out:Shipping Method</t>
-  </si>
-  <si>
     <t>accumulate</t>
   </si>
   <si>
@@ -69,24 +66,15 @@
     <t>$("Human Embryonic Stem Cell", "Human Embryonic Progenitor")</t>
   </si>
   <si>
-    <t>in:total_quantity</t>
-  </si>
-  <si>
     <t>out:Dry Ice Fee</t>
   </si>
   <si>
-    <t>out:Handling Fee</t>
-  </si>
-  <si>
     <t>$("Basal Media")</t>
   </si>
   <si>
     <t>2 day</t>
   </si>
   <si>
-    <t>$(BioTime)</t>
-  </si>
-  <si>
     <t>in:vendor_set</t>
   </si>
   <si>
@@ -94,6 +82,18 @@
   </si>
   <si>
     <t>in:pkg_quantity</t>
+  </si>
+  <si>
+    <t>out:BioTime Shipping Method</t>
+  </si>
+  <si>
+    <t>in:BioTime quantity</t>
+  </si>
+  <si>
+    <t>out:BioTime Handling</t>
+  </si>
+  <si>
+    <t>$(BioTime) &lt;= $in</t>
   </si>
 </sst>
 </file>
@@ -148,8 +148,8 @@
     </font>
     <font>
       <sz val="12"/>
-      <color indexed="72"/>
-      <name val="Lucida Grande"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="5">
@@ -196,7 +196,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="77">
+  <cellStyleXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -274,8 +274,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -287,8 +289,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="77">
+  <cellStyles count="79">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -327,6 +330,7 @@
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -365,6 +369,7 @@
     <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -414,7 +419,7 @@
             </a:prstGeom>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
@@ -422,6 +427,9 @@
               </a:pPr>
               <a:r>
                 <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
                   <a:latin typeface="Calibri"/>
                   <a:ea typeface="Calibri"/>
                   <a:cs typeface="Calibri"/>
@@ -765,65 +773,67 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A3" sqref="A3:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" customWidth="1"/>
+    <col min="1" max="1" width="21.83203125" customWidth="1"/>
     <col min="2" max="2" width="98.33203125" customWidth="1"/>
-    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" customWidth="1"/>
     <col min="4" max="4" width="13.83203125" customWidth="1"/>
-    <col min="5" max="7" width="19.5" customWidth="1"/>
+    <col min="5" max="5" width="25.83203125" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" customWidth="1"/>
+    <col min="7" max="7" width="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="39" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="10"/>
     </row>
     <row r="2" spans="1:12" s="3" customFormat="1">
       <c r="A2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" t="s">
-        <v>21</v>
+      <c r="A3" s="11" t="s">
+        <v>24</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -857,8 +867,8 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="16" thickBot="1">
-      <c r="A4" t="s">
-        <v>21</v>
+      <c r="A4" s="11" t="s">
+        <v>24</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -892,14 +902,14 @@
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" t="s">
-        <v>21</v>
+      <c r="A5" s="11" t="s">
+        <v>24</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8" t="s">
@@ -928,18 +938,18 @@
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" t="s">
-        <v>21</v>
+      <c r="A6" s="11" t="s">
+        <v>24</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F6" s="6">
         <v>0</v>
@@ -964,14 +974,14 @@
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" t="s">
-        <v>21</v>
+      <c r="A7" s="11" t="s">
+        <v>24</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6" t="s">
@@ -1000,18 +1010,18 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="16" thickBot="1">
-      <c r="A8" t="s">
-        <v>21</v>
+      <c r="A8" s="11" t="s">
+        <v>24</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F8" s="6">
         <v>0</v>
@@ -1036,14 +1046,14 @@
       </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" t="s">
-        <v>21</v>
+      <c r="A9" s="11" t="s">
+        <v>24</v>
       </c>
       <c r="B9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>7</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>8</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="8" t="s">
@@ -1072,14 +1082,14 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="16" thickBot="1">
-      <c r="A10" t="s">
-        <v>21</v>
+      <c r="A10" s="11" t="s">
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E10" t="s">
         <v>4</v>
@@ -1107,11 +1117,11 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="16" thickBot="1">
-      <c r="A11" t="s">
-        <v>21</v>
+      <c r="A11" s="11" t="s">
+        <v>24</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
@@ -1141,15 +1151,15 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="16" thickBot="1">
-      <c r="A12" t="s">
-        <v>21</v>
+      <c r="A12" s="11" t="s">
+        <v>24</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>4</v>
@@ -1177,14 +1187,14 @@
       </c>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" t="s">
-        <v>21</v>
+      <c r="A13" s="11" t="s">
+        <v>24</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E13" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
fixed bug in biotime_purchase_types
</commit_message>
<xml_diff>
--- a/rufus/carriers/lifemap_science/order/biotime_purchase_type.xlsx
+++ b/rufus/carriers/lifemap_science/order/biotime_purchase_type.xlsx
@@ -21,9 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="25">
   <si>
-    <t>in:product_types_set</t>
-  </si>
-  <si>
     <t>$("Growth Media")</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
     <t>in:vendor_set</t>
   </si>
   <si>
-    <t>$in intersection $(Differentiation Kit, Human Embryonic Progenitor Package, Growth Media, Basal Media) #&gt; 0</t>
-  </si>
-  <si>
     <t>in:pkg_quantity</t>
   </si>
   <si>
@@ -94,6 +88,12 @@
   </si>
   <si>
     <t>$(BioTime) &lt;= $in</t>
+  </si>
+  <si>
+    <t>in:biotime_product_types</t>
+  </si>
+  <si>
+    <t>$in intersection $(Differentiation Kit, Human Embryonic Progenitor Package, Growth Media, Basal Media) #&gt; 1</t>
   </si>
 </sst>
 </file>
@@ -773,7 +773,7 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A13"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -789,60 +789,60 @@
   <sheetData>
     <row r="1" spans="1:12" ht="39" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="10"/>
     </row>
     <row r="2" spans="1:12" s="3" customFormat="1">
       <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="E2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="H2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
       <c r="E3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F3">
         <v>1500</v>
@@ -868,16 +868,16 @@
     </row>
     <row r="4" spans="1:12" ht="16" thickBot="1">
       <c r="A4" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
         <v>3</v>
-      </c>
-      <c r="E4" t="s">
-        <v>4</v>
       </c>
       <c r="F4">
         <v>1500</v>
@@ -903,17 +903,17 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5" s="8">
         <v>0</v>
@@ -939,17 +939,17 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F6" s="6">
         <v>0</v>
@@ -975,17 +975,17 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7" s="6">
         <v>0</v>
@@ -1011,17 +1011,17 @@
     </row>
     <row r="8" spans="1:12" ht="16" thickBot="1">
       <c r="A8" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F8" s="6">
         <v>0</v>
@@ -1047,17 +1047,17 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B9" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>6</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>7</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F9" s="8">
         <v>1500</v>
@@ -1083,16 +1083,16 @@
     </row>
     <row r="10" spans="1:12" ht="16" thickBot="1">
       <c r="A10" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10">
         <v>1500</v>
@@ -1118,15 +1118,15 @@
     </row>
     <row r="11" spans="1:12" ht="16" thickBot="1">
       <c r="A11" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F11" s="8">
         <v>1500</v>
@@ -1152,17 +1152,17 @@
     </row>
     <row r="12" spans="1:12" ht="16" thickBot="1">
       <c r="A12" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>19</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F12" s="8">
         <v>1500</v>
@@ -1188,16 +1188,16 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>19</v>
-      </c>
       <c r="D13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F13">
         <v>1500</v>

</xml_diff>

<commit_message>
tweak to rules, which required rudelo bug fix
</commit_message>
<xml_diff>
--- a/rufus/carriers/lifemap_science/order/biotime_purchase_type.xlsx
+++ b/rufus/carriers/lifemap_science/order/biotime_purchase_type.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="26">
   <si>
     <t>$("Growth Media")</t>
   </si>
@@ -93,7 +93,10 @@
     <t>in:biotime_product_types</t>
   </si>
   <si>
-    <t>$in intersection $(Differentiation Kit, Human Embryonic Progenitor Package, Growth Media, Basal Media) #&gt; 1</t>
+    <t>$(Differentiation Kit, Human Embryonic Progenitor Package, Growth Media, Basal Media) &amp; $in #&gt; 0</t>
+  </si>
+  <si>
+    <t>#&gt; 1</t>
   </si>
 </sst>
 </file>
@@ -196,8 +199,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="79">
+  <cellStyleXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -291,7 +300,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="79">
+  <cellStyles count="85">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -331,6 +340,9 @@
     <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -370,6 +382,9 @@
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -770,30 +785,32 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="21.83203125" customWidth="1"/>
-    <col min="2" max="2" width="98.33203125" customWidth="1"/>
-    <col min="3" max="3" width="18.83203125" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" customWidth="1"/>
-    <col min="5" max="5" width="25.83203125" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" customWidth="1"/>
-    <col min="7" max="7" width="24" customWidth="1"/>
+    <col min="2" max="2" width="83.6640625" customWidth="1"/>
+    <col min="3" max="3" width="83.83203125" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" customWidth="1"/>
+    <col min="6" max="6" width="25.83203125" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" customWidth="1"/>
+    <col min="8" max="8" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="39" customHeight="1">
+    <row r="1" spans="1:13" ht="39" customHeight="1">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
     </row>
-    <row r="2" spans="1:12" s="3" customFormat="1">
+    <row r="2" spans="1:13" s="3" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -801,322 +818,330 @@
         <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:13">
       <c r="A3" s="11" t="s">
         <v>22</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>3</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>1500</v>
       </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3" s="5">
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="5">
         <v>2200</v>
       </c>
-      <c r="I3" s="5">
+      <c r="J3" s="5">
         <v>4900</v>
       </c>
-      <c r="J3" s="5">
+      <c r="K3" s="5">
         <v>5678</v>
       </c>
-      <c r="K3" s="5">
-        <v>5900</v>
-      </c>
       <c r="L3" s="5">
         <v>5900</v>
       </c>
+      <c r="M3" s="5">
+        <v>5900</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" ht="16" thickBot="1">
+    <row r="4" spans="1:13" ht="16" thickBot="1">
       <c r="A4" s="11" t="s">
         <v>22</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>3</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>1500</v>
       </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
       <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
         <v>2544</v>
       </c>
-      <c r="I4">
-        <v>5900</v>
-      </c>
       <c r="J4">
+        <v>5900</v>
+      </c>
+      <c r="K4">
         <v>6595</v>
-      </c>
-      <c r="K4">
-        <v>6900</v>
       </c>
       <c r="L4">
         <v>6900</v>
       </c>
+      <c r="M4">
+        <v>6900</v>
+      </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:13">
       <c r="A5" s="11" t="s">
         <v>22</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="8"/>
+      <c r="D5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="8"/>
+      <c r="F5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="8">
-        <v>0</v>
-      </c>
       <c r="G5" s="8">
         <v>0</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="8">
+        <v>0</v>
+      </c>
+      <c r="I5" s="9">
         <v>2200</v>
       </c>
-      <c r="I5" s="9">
+      <c r="J5" s="9">
         <v>4900</v>
       </c>
-      <c r="J5" s="9">
+      <c r="K5" s="9">
         <v>5678</v>
       </c>
-      <c r="K5" s="9">
-        <v>5900</v>
-      </c>
       <c r="L5" s="9">
         <v>5900</v>
       </c>
+      <c r="M5" s="9">
+        <v>5900</v>
+      </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:13">
       <c r="A6" s="11" t="s">
         <v>22</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="6"/>
+      <c r="D6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="6"/>
+      <c r="F6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="6">
-        <v>0</v>
-      </c>
       <c r="G6" s="6">
         <v>0</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="6">
+        <v>0</v>
+      </c>
+      <c r="I6" s="7">
         <v>1200</v>
       </c>
-      <c r="I6" s="7">
+      <c r="J6" s="7">
         <v>1563</v>
       </c>
-      <c r="J6" s="7">
+      <c r="K6" s="7">
         <v>2233</v>
       </c>
-      <c r="K6" s="7">
+      <c r="L6" s="7">
         <v>3590</v>
       </c>
-      <c r="L6" s="7">
+      <c r="M6" s="7">
         <v>3744</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:13">
       <c r="A7" s="11" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="6"/>
+      <c r="D7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="6"/>
+      <c r="F7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="6">
-        <v>0</v>
-      </c>
       <c r="G7" s="6">
         <v>0</v>
       </c>
       <c r="H7" s="6">
+        <v>0</v>
+      </c>
+      <c r="I7" s="6">
         <v>2544</v>
       </c>
-      <c r="I7" s="6">
-        <v>5900</v>
-      </c>
       <c r="J7" s="6">
+        <v>5900</v>
+      </c>
+      <c r="K7" s="6">
         <v>6595</v>
       </c>
-      <c r="K7" s="6">
+      <c r="L7" s="6">
         <v>7436</v>
       </c>
-      <c r="L7" s="6">
+      <c r="M7" s="6">
         <v>7855</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="16" thickBot="1">
+    <row r="8" spans="1:13" ht="16" thickBot="1">
       <c r="A8" s="11" t="s">
         <v>22</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="6"/>
+      <c r="D8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="6"/>
+      <c r="F8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="6">
-        <v>0</v>
-      </c>
       <c r="G8" s="6">
         <v>0</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="6">
+        <v>0</v>
+      </c>
+      <c r="I8" s="7">
         <v>1500</v>
       </c>
-      <c r="I8" s="7">
+      <c r="J8" s="7">
         <v>2000</v>
       </c>
-      <c r="J8" s="7">
+      <c r="K8" s="7">
         <v>2745</v>
       </c>
-      <c r="K8" s="7">
+      <c r="L8" s="7">
         <v>4565</v>
       </c>
-      <c r="L8" s="7">
+      <c r="M8" s="7">
         <v>4728</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:13">
       <c r="A9" s="11" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="8"/>
+      <c r="D9" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="8"/>
+      <c r="F9" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="8">
+      <c r="G9" s="8">
         <v>1500</v>
       </c>
-      <c r="G9" s="8">
-        <v>0</v>
-      </c>
-      <c r="H9" s="9">
+      <c r="H9" s="8">
+        <v>0</v>
+      </c>
+      <c r="I9" s="9">
         <v>2200</v>
       </c>
-      <c r="I9" s="9">
+      <c r="J9" s="9">
         <v>4900</v>
       </c>
-      <c r="J9" s="9">
+      <c r="K9" s="9">
         <v>5678</v>
       </c>
-      <c r="K9" s="9">
-        <v>5900</v>
-      </c>
       <c r="L9" s="9">
         <v>5900</v>
       </c>
+      <c r="M9" s="9">
+        <v>5900</v>
+      </c>
     </row>
-    <row r="10" spans="1:12" ht="16" thickBot="1">
+    <row r="10" spans="1:13" ht="16" thickBot="1">
       <c r="A10" s="11" t="s">
         <v>22</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>7</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>3</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>1500</v>
       </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10" s="5">
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10" s="5">
         <v>2544</v>
       </c>
-      <c r="I10" s="5">
-        <v>5900</v>
-      </c>
       <c r="J10" s="5">
+        <v>5900</v>
+      </c>
+      <c r="K10" s="5">
         <v>6595</v>
-      </c>
-      <c r="K10" s="5">
-        <v>6900</v>
       </c>
       <c r="L10" s="5">
         <v>6900</v>
       </c>
+      <c r="M10" s="5">
+        <v>6900</v>
+      </c>
     </row>
-    <row r="11" spans="1:12" ht="16" thickBot="1">
+    <row r="11" spans="1:13" ht="16" thickBot="1">
       <c r="A11" s="11" t="s">
         <v>22</v>
       </c>
@@ -1125,99 +1150,106 @@
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="8"/>
+      <c r="F11" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F11" s="8">
+      <c r="G11" s="8">
         <v>1500</v>
       </c>
-      <c r="G11" s="8">
-        <v>0</v>
-      </c>
-      <c r="H11" s="9">
+      <c r="H11" s="8">
+        <v>0</v>
+      </c>
+      <c r="I11" s="9">
         <v>2200</v>
       </c>
-      <c r="I11" s="9">
+      <c r="J11" s="9">
         <v>4900</v>
       </c>
-      <c r="J11" s="9">
+      <c r="K11" s="9">
         <v>5678</v>
       </c>
-      <c r="K11" s="9">
-        <v>5900</v>
-      </c>
       <c r="L11" s="9">
         <v>5900</v>
       </c>
+      <c r="M11" s="9">
+        <v>5900</v>
+      </c>
     </row>
-    <row r="12" spans="1:12" ht="16" thickBot="1">
+    <row r="12" spans="1:13">
       <c r="A12" s="11" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8" t="s">
+      <c r="C12" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="F12" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F12" s="8">
+      <c r="G12" s="8">
         <v>1500</v>
       </c>
-      <c r="G12" s="8">
-        <v>0</v>
-      </c>
-      <c r="H12" s="9">
+      <c r="H12" s="8">
+        <v>0</v>
+      </c>
+      <c r="I12" s="9">
         <v>2200</v>
       </c>
-      <c r="I12" s="9">
+      <c r="J12" s="9">
         <v>4900</v>
       </c>
-      <c r="J12" s="9">
+      <c r="K12" s="9">
         <v>5678</v>
       </c>
-      <c r="K12" s="9">
-        <v>5900</v>
-      </c>
       <c r="L12" s="9">
         <v>5900</v>
       </c>
+      <c r="M12" s="9">
+        <v>5900</v>
+      </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:13">
       <c r="A13" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" t="s">
         <v>24</v>
       </c>
-      <c r="D13" t="s">
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" t="s">
         <v>7</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>3</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>1500</v>
       </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
       <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
         <v>2544</v>
       </c>
-      <c r="I13">
-        <v>5900</v>
-      </c>
       <c r="J13">
+        <v>5900</v>
+      </c>
+      <c r="K13">
         <v>6595</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>6900</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>6900</v>
       </c>
     </row>

</xml_diff>